<commit_message>
modified:   .DS_Store 	modified:   data/processed/autoscout_clean_ml.xlsx 	modified:   data/processed/voitures_nettoyees.json 	deleted:    data/processed/~$autoscout_clean_ml.xlsx 	modified:   models/comparaison_modeles.xlsx 	new file:   src/__pycache__/MachineLearning.cpython-312.pyc 	new file:   src/__pycache__/cleaning.cpython-312.pyc 	modified:   src/cleaning.py
</commit_message>
<xml_diff>
--- a/models/comparaison_modeles.xlsx
+++ b/models/comparaison_modeles.xlsx
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>€9,724.01</t>
+          <t>€27,144.34</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>€8,974.31</t>
+          <t>€27,459.02</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.8302</t>
+          <t>-1650788376.1205</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.8554</t>
+          <t>-1689285588.1029</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>€4,459.42</t>
+          <t>€22,130.19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>€4,183.93</t>
+          <t>€22,360.75</t>
         </is>
       </c>
     </row>

</xml_diff>